<commit_message>
modelo 1 conatntes para 12 seroencuestas
</commit_message>
<xml_diff>
--- a/WAIC_colHPV18.xlsx
+++ b/WAIC_colHPV18.xlsx
@@ -12,15 +12,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
   <si>
     <t xml:space="preserve">constant</t>
   </si>
   <si>
     <t xml:space="preserve">normal</t>
-  </si>
-  <si>
-    <t xml:space="preserve">normal_log_HPV18col</t>
   </si>
 </sst>
 </file>
@@ -359,9 +356,6 @@
       <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
@@ -370,9 +364,6 @@
       <c r="B2" t="n">
         <v>61.5749989056075</v>
       </c>
-      <c r="C2" t="n">
-        <v>45.3857335469521</v>
-      </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
@@ -380,9 +371,6 @@
       </c>
       <c r="B3" t="n">
         <v>13.8810302415049</v>
-      </c>
-      <c r="C3" t="n">
-        <v>6.62577701693813</v>
       </c>
     </row>
   </sheetData>

</xml_diff>